<commit_message>
Tout fonctionne sauf redirection et pré-remplissage des formulaires
Le bouton 'Double création' insère correctement l’écriture mais réaffiche le formulaire vide au lieu d’un popup ; les clics sur les numéros d’écriture renvoient le mauvais template (fournisseurs vs. comptabilité) et ne sont pas pré-remplis.
</commit_message>
<xml_diff>
--- a/bd_factures_fournisseurs.xlsx
+++ b/bd_factures_fournisseurs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X60"/>
+  <dimension ref="A1:X63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6505,6 +6505,344 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Fournisseur_02</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1001 – Caisse 2</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>31 jours</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2025-07-24</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>1010 – CCP 1</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>test24</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>132.00</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>test24</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>136.00</t>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>1012</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Fournisseur_07</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1100 – Débiteurs 1</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>36 jours</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>1101 – Débiteurs 2</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>909.00</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>1200 – Stock 1</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>921.00</t>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>1013</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Fournisseur_03</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1010 – CCP 1</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>32 jours</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>1056.00</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>1091.00</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>1014</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
numéro décriture renvoie toujours le même form ecriture manuelle
</commit_message>
<xml_diff>
--- a/bd_factures_fournisseurs.xlsx
+++ b/bd_factures_fournisseurs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X63"/>
+  <dimension ref="A1:X80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6843,6 +6843,1256 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Fournisseur_05</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>34 jours</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>81000000.00</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>1100 – Débiteurs 1</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>81009000.00</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>1015</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Fournisseur_03</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1010 – CCP 1</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>32 jours</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>64000000.00</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>64008000.00</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>1016</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Fournisseur_07</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1100 – Débiteurs 1</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>36 jours</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2025-07-26</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>1101 – Débiteurs 2</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>400.00</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>1200 – Stock 1</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>420.00</t>
+        </is>
+      </c>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>1017</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Fournisseur_04</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>33 jours</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2025-07-26</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>9000000.00</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>9003000.00</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>1018</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Fournisseur_04</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>33 jours</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>10000.00</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Fournisseur_04</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>33 jours</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2025-07-26</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr"/>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>7.7</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>12000.00</t>
+        </is>
+      </c>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>1020</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Fournisseur_10</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1201 – Stock2</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>39 jours</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>1300 – Actif transitoire 1</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>1301 – Actif transitoire 2</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>1021</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Fournisseur_03</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1010 – CCP 1</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>32 jours</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>1022</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Fournisseur_06</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>35 jours</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>1100 – Débiteurs 1</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>1101 – Débiteurs 2</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr"/>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>1023</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Fournisseur_04</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>33 jours</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>1024</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Fournisseur_07</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1100 – Débiteurs 1</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>36 jours</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>1101 – Débiteurs 2</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>1200 – Stock 1</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr"/>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Fournisseur_10</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1201 – Stock2</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>39 jours</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2025-07</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>1300 – Actif transitoire 1</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>1301 – Actif transitoire 2</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr"/>
+      <c r="T75" t="inlineStr"/>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>1026</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Fournisseur_02</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1001 – Caisse 2</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>31 jours</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>1010 – CCP 1</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr"/>
+      <c r="T76" t="inlineStr"/>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr"/>
+      <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>1027</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Fournisseur_05</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>34 jours</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>1100 – Débiteurs 1</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr"/>
+      <c r="T77" t="inlineStr"/>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>1028</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1011 – CCP 2</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>33 jours</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>1020 – Banque 1</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>1021 – Banque 2</t>
+        </is>
+      </c>
+      <c r="S78" t="inlineStr"/>
+      <c r="T78" t="inlineStr"/>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr"/>
+      <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>1029</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Fournisseur_08</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1101 – Débiteurs 2</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>37 jours</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2025-07-26</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>1200 – Stock 1</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>1201 – Stock2</t>
+        </is>
+      </c>
+      <c r="S79" t="inlineStr"/>
+      <c r="T79" t="inlineStr"/>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V79" t="inlineStr"/>
+      <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>1030</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
+      <c r="R80" t="inlineStr"/>
+      <c r="S80" t="inlineStr"/>
+      <c r="T80" t="inlineStr"/>
+      <c r="U80" t="inlineStr"/>
+      <c r="V80" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>1031</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>